<commit_message>
push tableau to streamlit
</commit_message>
<xml_diff>
--- a/data/mcdonalds_prices.xlsx
+++ b/data/mcdonalds_prices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Github/would_you_like_some_fries_with_that/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86926BCC-1C20-F346-B8B8-0EC4632752C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C34B0C5-377F-1A41-8461-853184941400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="660" windowWidth="12800" windowHeight="15980" xr2:uid="{481F8FB7-0DD3-7A40-8F87-D41B6690285B}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="15980" xr2:uid="{481F8FB7-0DD3-7A40-8F87-D41B6690285B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet3" sheetId="3" r:id="rId1"/>
@@ -53,51 +53,12 @@
     <t>Triple Cheeseburger</t>
   </si>
   <si>
-    <t>Double Quarter Pounder¬Æ with Cheese</t>
-  </si>
-  <si>
-    <t>Quarter Pounder¬Æ with Cheese</t>
-  </si>
-  <si>
-    <t>Big Mac¬Æ</t>
-  </si>
-  <si>
     <t>Double Cheeseburger</t>
   </si>
   <si>
-    <t>Chicken McCrispy¬Æ (2pc)</t>
-  </si>
-  <si>
     <t>Buttermilk Crispy Chicken</t>
   </si>
   <si>
-    <t>Double McSpicy¬Æ</t>
-  </si>
-  <si>
-    <t>McSpicy¬Æ</t>
-  </si>
-  <si>
-    <t>Double Filet-O-Fish¬Æ</t>
-  </si>
-  <si>
-    <t>Filet-O-Fish¬Æ</t>
-  </si>
-  <si>
-    <t>Chicken McNuggets¬Æ (9pc)</t>
-  </si>
-  <si>
-    <t>Chicken McNuggets¬Æ (6pc)</t>
-  </si>
-  <si>
-    <t>McWings¬Æ (4pc)</t>
-  </si>
-  <si>
-    <t>McChicken¬Æ</t>
-  </si>
-  <si>
-    <t>Grilled Chicken McWrap¬Æ</t>
-  </si>
-  <si>
     <t>Grilled Chicken Salad</t>
   </si>
   <si>
@@ -113,9 +74,6 @@
     <t>Ala Carte</t>
   </si>
   <si>
-    <t>Chicken McCrispy¬Æ (6pc)</t>
-  </si>
-  <si>
     <t>Apple Custard Pie</t>
   </si>
   <si>
@@ -125,9 +83,6 @@
     <t>French Fries (Small)</t>
   </si>
   <si>
-    <t>Chicken McNuggets¬Æ (20pc)</t>
-  </si>
-  <si>
     <t>Apple Slices</t>
   </si>
   <si>
@@ -137,30 +92,15 @@
     <t>Corn Cup (5oz)</t>
   </si>
   <si>
-    <t>McWings¬Æ (2pc)</t>
-  </si>
-  <si>
     <t>Lotus Biscoff McFlurry</t>
   </si>
   <si>
-    <t>OREO¬Æ McFlurry¬Æ</t>
-  </si>
-  <si>
-    <t>Mudpie McFlurry¬Æ</t>
-  </si>
-  <si>
-    <t>Strawberry Shortcake McFlurry¬Æ</t>
-  </si>
-  <si>
     <t>Hot Fudge Sundae</t>
   </si>
   <si>
     <t>Strawberry Sundae</t>
   </si>
   <si>
-    <t>ChocoCone¬Æ</t>
-  </si>
-  <si>
     <t>Vanilla Cone</t>
   </si>
   <si>
@@ -173,33 +113,12 @@
     <t>Mocha Frappe with Oreo</t>
   </si>
   <si>
-    <t>Caramel Frapp√© (Small)</t>
-  </si>
-  <si>
-    <t>Mocha Frapp√© (Small)</t>
-  </si>
-  <si>
-    <t>Iced MILO¬Æ (Small)</t>
-  </si>
-  <si>
     <t>Jasmine Green Tea (Small)</t>
   </si>
   <si>
     <t>Iced Lemon Tea (Small)</t>
   </si>
   <si>
-    <t>McCaf√©¬Æ Cappuccino</t>
-  </si>
-  <si>
-    <t>McCaf√©¬Æ Latte</t>
-  </si>
-  <si>
-    <t>McCaf√© Iced Latte</t>
-  </si>
-  <si>
-    <t>McCaf√©¬Æ Premium Roast Coffee</t>
-  </si>
-  <si>
     <t>100% Pure Orange Juice (Small)</t>
   </si>
   <si>
@@ -209,18 +128,6 @@
     <t>Hot Tea</t>
   </si>
   <si>
-    <t>Hot MILO¬Æ</t>
-  </si>
-  <si>
-    <t>Coca-Cola¬Æ Zero Sugar (Small)</t>
-  </si>
-  <si>
-    <t>Coca-Cola¬Æ Original Taste Less Sugar (Small)</t>
-  </si>
-  <si>
-    <t>Sprite¬Æ (Small)</t>
-  </si>
-  <si>
     <t>Dasani</t>
   </si>
   <si>
@@ -242,9 +149,6 @@
     <t>Breakfast Deluxe</t>
   </si>
   <si>
-    <t>Big Breakfast¬Æ</t>
-  </si>
-  <si>
     <t>Breakfast Wrap Chicken Sausage</t>
   </si>
   <si>
@@ -257,21 +161,12 @@
     <t>Hotcakes</t>
   </si>
   <si>
-    <t>Sausage McMuffin¬Æ</t>
-  </si>
-  <si>
-    <t>Sausage McMuffin¬Æ with Egg</t>
-  </si>
-  <si>
     <t>Chicken Muffin with Egg</t>
   </si>
   <si>
     <t>Chicken Muffin</t>
   </si>
   <si>
-    <t>Egg McMuffin¬Æ</t>
-  </si>
-  <si>
     <t>Hash Brown</t>
   </si>
   <si>
@@ -284,13 +179,118 @@
     <t>Classification</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
+    <t>Double Quarter Pounder with Cheese</t>
+  </si>
+  <si>
+    <t>Quarter Pounder with Cheese</t>
+  </si>
+  <si>
+    <t>Big Mac</t>
+  </si>
+  <si>
+    <t>Chicken McCrispy (2pc)</t>
+  </si>
+  <si>
+    <t>Double McSpicy</t>
+  </si>
+  <si>
+    <t>McSpicy</t>
+  </si>
+  <si>
+    <t>Double Filet-O-Fish</t>
+  </si>
+  <si>
+    <t>Filet-O-Fish</t>
+  </si>
+  <si>
+    <t>Chicken McNuggets (9pc)</t>
+  </si>
+  <si>
+    <t>Chicken McNuggets (6pc)</t>
+  </si>
+  <si>
+    <t>McWings (4pc)</t>
+  </si>
+  <si>
+    <t>McChicken</t>
+  </si>
+  <si>
+    <t>Grilled Chicken McWrap</t>
+  </si>
+  <si>
+    <t>Chicken McCrispy (6pc)</t>
+  </si>
+  <si>
+    <t>Chicken McNuggets (20pc)</t>
+  </si>
+  <si>
+    <t>McWings (2pc)</t>
+  </si>
+  <si>
+    <t>OREO McFlurry</t>
+  </si>
+  <si>
+    <t>Mudpie McFlurry</t>
+  </si>
+  <si>
+    <t>Strawberry Shortcake McFlurry</t>
+  </si>
+  <si>
+    <t>ChocoCone</t>
+  </si>
+  <si>
+    <t>Iced MILO (Small)</t>
+  </si>
+  <si>
+    <t>Hot MILO</t>
+  </si>
+  <si>
+    <t>Coca-Cola Zero Sugar (Small)</t>
+  </si>
+  <si>
+    <t>Coca-Cola Original Taste Less Sugar (Small)</t>
+  </si>
+  <si>
+    <t>Sprite (Small)</t>
+  </si>
+  <si>
+    <t>Big Breakfast</t>
+  </si>
+  <si>
+    <t>Sausage McMuffin</t>
+  </si>
+  <si>
+    <t>Sausage McMuffin with Egg</t>
+  </si>
+  <si>
+    <t>Egg McMuffin</t>
+  </si>
+  <si>
+    <t>Caramel Frappe (Small)</t>
+  </si>
+  <si>
+    <t>Mocha Frappe (Small)</t>
+  </si>
+  <si>
+    <t>McCafe Cappuccino</t>
+  </si>
+  <si>
+    <t>McCafe Latte</t>
+  </si>
+  <si>
+    <t>McCafe Iced Latte</t>
+  </si>
+  <si>
+    <t>McCafe Premium Roast Coffee</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>High</t>
   </si>
 </sst>
 </file>
@@ -654,7 +654,7 @@
   <dimension ref="A1:G129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,13 +666,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>82</v>
@@ -684,7 +684,7 @@
         <v>84</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>80</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -715,7 +715,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C3">
         <v>9.9</v>
@@ -738,7 +738,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C4">
         <v>8.3000000000000007</v>
@@ -761,7 +761,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C5">
         <v>8.6</v>
@@ -784,7 +784,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>7.3</v>
@@ -807,7 +807,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -830,7 +830,7 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -853,7 +853,7 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <v>9.9</v>
@@ -876,7 +876,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C10">
         <v>9.4499999999999993</v>
@@ -899,7 +899,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C11">
         <v>8.1999999999999993</v>
@@ -922,7 +922,7 @@
         <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C12">
         <v>8.1999999999999993</v>
@@ -945,7 +945,7 @@
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="C13">
         <v>6.6</v>
@@ -968,7 +968,7 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C14">
         <v>9.1</v>
@@ -991,7 +991,7 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C15">
         <v>7.8</v>
@@ -1014,7 +1014,7 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C16">
         <v>7.5</v>
@@ -1037,7 +1037,7 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D17">
         <v>6.9</v>
@@ -1054,7 +1054,7 @@
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C18">
         <v>8.15</v>
@@ -1077,7 +1077,7 @@
         <v>3</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C19">
         <v>8.15</v>
@@ -1100,7 +1100,7 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D20">
         <v>6.45</v>
@@ -1117,7 +1117,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D21">
         <v>6.05</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C23">
         <v>8.9</v>
@@ -1177,10 +1177,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C24">
         <v>7.3</v>
@@ -1200,10 +1200,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C25">
         <v>7.6</v>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>6.3</v>
@@ -1246,10 +1246,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C27">
         <v>8</v>
@@ -1269,10 +1269,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C28">
         <v>8</v>
@@ -1292,10 +1292,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C29">
         <v>8.9</v>
@@ -1315,10 +1315,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C30">
         <v>8.4499999999999993</v>
@@ -1338,10 +1338,10 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C31">
         <v>7.2</v>
@@ -1361,10 +1361,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C32">
         <v>7.2</v>
@@ -1384,10 +1384,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="C33">
         <v>5.6</v>
@@ -1407,10 +1407,10 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C34">
         <v>8.1</v>
@@ -1430,10 +1430,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C35">
         <v>6.8</v>
@@ -1453,10 +1453,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C36">
         <v>6.5</v>
@@ -1476,10 +1476,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="D37">
         <v>5.9</v>
@@ -1493,10 +1493,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C38">
         <v>7.15</v>
@@ -1516,10 +1516,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C39">
         <v>7.15</v>
@@ -1539,10 +1539,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D40">
         <v>5.45</v>
@@ -1556,10 +1556,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D41">
         <v>5.05</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B42" t="s">
         <v>4</v>
@@ -1596,10 +1596,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="C43">
         <v>7.3</v>
@@ -1619,10 +1619,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C44">
         <v>5.7</v>
@@ -1642,10 +1642,10 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C45">
         <v>5.6</v>
@@ -1665,10 +1665,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C46">
         <v>3.9</v>
@@ -1688,10 +1688,10 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="C47">
         <v>6.8</v>
@@ -1711,10 +1711,10 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="C48">
         <v>18.8</v>
@@ -1734,10 +1734,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C49">
         <v>6.9</v>
@@ -1757,10 +1757,10 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>11</v>
+        <v>51</v>
       </c>
       <c r="C50">
         <v>7.2</v>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="C51">
         <v>6.3</v>
@@ -1803,10 +1803,10 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B52" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C52">
         <v>5.45</v>
@@ -1826,10 +1826,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="C53">
         <v>3.35</v>
@@ -1849,10 +1849,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B54" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="C54">
         <v>6.8</v>
@@ -1872,10 +1872,10 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B55" t="s">
-        <v>16</v>
+        <v>56</v>
       </c>
       <c r="C55">
         <v>5.4</v>
@@ -1895,10 +1895,10 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B56" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C56">
         <v>2.8</v>
@@ -1918,10 +1918,10 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B57" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="C57">
         <v>2.25</v>
@@ -1941,10 +1941,10 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B58" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C58">
         <v>5.35</v>
@@ -1964,10 +1964,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C59">
         <v>5.35</v>
@@ -1987,10 +1987,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B60" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C60">
         <v>2.1</v>
@@ -2013,7 +2013,7 @@
         <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C61">
         <v>1.8</v>
@@ -2036,7 +2036,7 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C62">
         <v>3.6</v>
@@ -2059,7 +2059,7 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C63">
         <v>1.9</v>
@@ -2082,7 +2082,7 @@
         <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="C64">
         <v>4.05</v>
@@ -2105,7 +2105,7 @@
         <v>1</v>
       </c>
       <c r="B65" t="s">
-        <v>29</v>
+        <v>61</v>
       </c>
       <c r="C65">
         <v>11.65</v>
@@ -2128,7 +2128,7 @@
         <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C66">
         <v>1.9</v>
@@ -2151,7 +2151,7 @@
         <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="C67">
         <v>1.4</v>
@@ -2174,7 +2174,7 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C68">
         <v>1.6</v>
@@ -2197,7 +2197,7 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="C69">
         <v>2.6</v>
@@ -2220,7 +2220,7 @@
         <v>0</v>
       </c>
       <c r="B70" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C70">
         <v>3.5</v>
@@ -2243,7 +2243,7 @@
         <v>0</v>
       </c>
       <c r="B71" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="C71">
         <v>2.95</v>
@@ -2266,7 +2266,7 @@
         <v>0</v>
       </c>
       <c r="B72" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="C72">
         <v>3.25</v>
@@ -2289,7 +2289,7 @@
         <v>0</v>
       </c>
       <c r="B73" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C73">
         <v>3.25</v>
@@ -2312,7 +2312,7 @@
         <v>0</v>
       </c>
       <c r="B74" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C74">
         <v>2</v>
@@ -2335,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="B75" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C75">
         <v>2</v>
@@ -2358,7 +2358,7 @@
         <v>0</v>
       </c>
       <c r="B76" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="C76">
         <v>1.2</v>
@@ -2381,7 +2381,7 @@
         <v>0</v>
       </c>
       <c r="B77" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C77">
         <v>1</v>
@@ -2401,10 +2401,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C78">
         <v>4.2</v>
@@ -2424,10 +2424,10 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B79" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="C79">
         <v>4.2</v>
@@ -2447,10 +2447,10 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B80" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="C80">
         <v>3.8</v>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B81" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C81">
         <v>3.8</v>
@@ -2493,10 +2493,10 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B82" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="C82">
         <v>3.5</v>
@@ -2516,10 +2516,10 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B83" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C83">
         <v>3.4</v>
@@ -2539,10 +2539,10 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B84" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C84">
         <v>3.4</v>
@@ -2562,10 +2562,10 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B85" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="C85">
         <v>3.7</v>
@@ -2585,10 +2585,10 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B86" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="C86">
         <v>3.7</v>
@@ -2608,10 +2608,10 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B87" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="C87">
         <v>3.9</v>
@@ -2631,10 +2631,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B88" t="s">
-        <v>53</v>
+        <v>81</v>
       </c>
       <c r="C88">
         <v>2.7</v>
@@ -2654,10 +2654,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B89" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="C89">
         <v>3.55</v>
@@ -2677,10 +2677,10 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B90" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C90">
         <v>2.6</v>
@@ -2700,10 +2700,10 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B91" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C91">
         <v>2.7</v>
@@ -2723,10 +2723,10 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B92" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="C92">
         <v>2.75</v>
@@ -2746,10 +2746,10 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B93" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C93">
         <v>2.8</v>
@@ -2769,10 +2769,10 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B94" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C94">
         <v>2.8</v>
@@ -2792,10 +2792,10 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B95" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C95">
         <v>2.8</v>
@@ -2815,10 +2815,10 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B96" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="C96">
         <v>2.4500000000000002</v>
@@ -2838,10 +2838,10 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B97" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="D97">
         <v>6.8</v>
@@ -2855,10 +2855,10 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B98" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="D98">
         <v>6.8</v>
@@ -2872,10 +2872,10 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B99" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="D99">
         <v>7.9</v>
@@ -2889,10 +2889,10 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B100" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="D100">
         <v>5.9</v>
@@ -2906,10 +2906,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B101" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="D101">
         <v>8.8000000000000007</v>
@@ -2923,10 +2923,10 @@
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B102" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D102">
         <v>7.35</v>
@@ -2940,10 +2940,10 @@
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B103" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D103">
         <v>6.7</v>
@@ -2957,10 +2957,10 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B104" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="D104">
         <v>6.25</v>
@@ -2974,10 +2974,10 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B105" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="D105">
         <v>8.1</v>
@@ -2991,10 +2991,10 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B106" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="D106">
         <v>7.15</v>
@@ -3008,7 +3008,7 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B107" t="s">
         <v>73</v>
@@ -3025,7 +3025,7 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B108" t="s">
         <v>74</v>
@@ -3042,10 +3042,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B109" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="D109">
         <v>5.85</v>
@@ -3059,10 +3059,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B110" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="D110">
         <v>5</v>
@@ -3076,10 +3076,10 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B111" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D111">
         <v>5</v>
@@ -3093,10 +3093,10 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B112" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="D112">
         <v>7.9</v>
@@ -3110,10 +3110,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="B113" t="s">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="D113">
         <v>6.15</v>
@@ -3127,10 +3127,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B114" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C114">
         <v>6.2</v>
@@ -3150,10 +3150,10 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B115" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="C115">
         <v>6.2</v>
@@ -3173,10 +3173,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B116" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="C116">
         <v>7</v>
@@ -3196,10 +3196,10 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B117" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="C117">
         <v>5.3</v>
@@ -3219,10 +3219,10 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B118" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C118">
         <v>6.55</v>
@@ -3242,10 +3242,10 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B119" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C119">
         <v>5.55</v>
@@ -3265,10 +3265,10 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B120" t="s">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="C120">
         <v>4.95</v>
@@ -3288,10 +3288,10 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B121" t="s">
-        <v>70</v>
+        <v>38</v>
       </c>
       <c r="C121">
         <v>4.5</v>
@@ -3311,10 +3311,10 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B122" t="s">
-        <v>71</v>
+        <v>39</v>
       </c>
       <c r="C122">
         <v>5.9</v>
@@ -3334,10 +3334,10 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B123" t="s">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="C123">
         <v>4.9000000000000004</v>
@@ -3357,7 +3357,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B124" t="s">
         <v>74</v>
@@ -3380,7 +3380,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B125" t="s">
         <v>73</v>
@@ -3403,10 +3403,10 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B126" t="s">
-        <v>75</v>
+        <v>41</v>
       </c>
       <c r="C126">
         <v>3.7</v>
@@ -3426,10 +3426,10 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B127" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="C127">
         <v>2.9</v>
@@ -3449,10 +3449,10 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B128" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C128">
         <v>3.7</v>
@@ -3475,7 +3475,7 @@
         <v>1</v>
       </c>
       <c r="B129" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="C129">
         <v>2.25</v>

</xml_diff>